<commit_message>
just looking at JD's/added sheet in xls
</commit_message>
<xml_diff>
--- a/PCA_layout_for_naming.xlsx
+++ b/PCA_layout_for_naming.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Documents\Schooling\Willamette-MSDS\2-DATA505_MachineLearning\Project_2\repo\ML-Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaacjohnson/Documents/Scanner Output/School/Willamette/Machine Learning/Week 10/Project 2/Git_Project2/ML-Project2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741DA96A-4792-4FF7-8A37-9719B72FAD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21E8D84-CB08-1A4D-A2DD-727F584DDBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BAF7EC1-6934-4E82-A88D-5BFC29E54102}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26700" windowHeight="16920" activeTab="1" xr2:uid="{7BAF7EC1-6934-4E82-A88D-5BFC29E54102}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'v2'!$A$1:$G$31</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
   <si>
     <t>PC1</t>
   </si>
@@ -189,6 +193,90 @@
   </si>
   <si>
     <t>Top five for fetaures</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>- blue -.37</t>
+  </si>
+  <si>
+    <t>- gender -.49</t>
+  </si>
+  <si>
+    <t>income +.49</t>
+  </si>
+  <si>
+    <t>silver +.35</t>
+  </si>
+  <si>
+    <t>- Total_Revolving_Bal -.48</t>
+  </si>
+  <si>
+    <t>-Avg_Utilization_Ratio -0.40</t>
+  </si>
+  <si>
+    <t>- married -.60</t>
+  </si>
+  <si>
+    <t>- Total_Revolving_Bal -.31</t>
+  </si>
+  <si>
+    <t>single +.58</t>
+  </si>
+  <si>
+    <t>- Total_Amt_Chng_Q4_Q1 -.23</t>
+  </si>
+  <si>
+    <t>-Total Relationship Count -0.31</t>
+  </si>
+  <si>
+    <t>-single -.29</t>
+  </si>
+  <si>
+    <t>Customer_Age +.65</t>
+  </si>
+  <si>
+    <t>Months_on_book +.64</t>
+  </si>
+  <si>
+    <t>- Dependent_count -.16</t>
+  </si>
+  <si>
+    <t>Total_Trans_Amt +.16</t>
+  </si>
+  <si>
+    <t>Total_Trans_Ct +.52</t>
+  </si>
+  <si>
+    <t>Total_Trans_Amt +.48</t>
+  </si>
+  <si>
+    <t>- Total_Relationship_Count -.24</t>
+  </si>
+  <si>
+    <t>- gender -.24</t>
+  </si>
+  <si>
+    <t>- Avg_Open_To_Buy -.47</t>
+  </si>
+  <si>
+    <t>- Credit_Limit -.47</t>
+  </si>
+  <si>
+    <t>- silver -.34</t>
+  </si>
+  <si>
+    <t>blue +.39</t>
+  </si>
+  <si>
+    <t>Avg Open to Buy</t>
+  </si>
+  <si>
+    <t>single/Married</t>
+  </si>
+  <si>
+    <t>income/gender?</t>
   </si>
 </sst>
 </file>
@@ -265,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -276,6 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,23 +681,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49EB4EE4-2F6D-4B8C-8F30-3514F7F0C1A4}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -651,7 +740,7 @@
         <v>-6.0063233000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -674,7 +763,7 @@
         <v>1.6327528000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -697,7 +786,7 @@
         <v>-6.5670746000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -720,7 +809,7 @@
         <v>1.6978592000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -743,7 +832,7 @@
         <v>6.4796257999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -766,7 +855,7 @@
         <v>8.4352883000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -789,7 +878,7 @@
         <v>-6.5254820000000005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -812,7 +901,7 @@
         <v>-0.161380367</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -835,7 +924,7 @@
         <v>-5.0773237999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -858,7 +947,7 @@
         <v>-0.21017197000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -881,7 +970,7 @@
         <v>-0.12641769899999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -904,7 +993,7 @@
         <v>-0.115756189</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -927,7 +1016,7 @@
         <v>-0.24298362000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -950,7 +1039,7 @@
         <v>-3.6143762000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -973,7 +1062,7 @@
         <v>-0.48653523199999998</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -996,7 +1085,7 @@
         <v>0.17015984200000001</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1019,7 +1108,7 @@
         <v>-0.17971151799999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1042,7 +1131,7 @@
         <v>5.7594359999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1065,7 +1154,7 @@
         <v>4.8806780000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1088,7 +1177,7 @@
         <v>-0.36689286700000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1111,7 +1200,7 @@
         <v>8.2550703000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1134,7 +1223,7 @@
         <v>0.358475818</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1157,7 +1246,7 @@
         <v>4.8161047999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1180,7 +1269,7 @@
         <v>-4.7152468000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1203,14 +1292,14 @@
         <v>0.49085000699999998</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="H27" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1236,7 +1325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1262,7 +1351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
@@ -1308,12 +1397,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H32" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -1333,71 +1422,71 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
     </row>
   </sheetData>
@@ -1407,4 +1496,839 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F67C65-8765-BE4A-A3F4-4849C74ABCB4}">
+  <dimension ref="A1:H60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3">
+        <v>-0.4702684325</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.13203382499999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-1.9647541000000001E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-1.8914360000000002E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-1.9767716000000001E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-5.0773237999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-0.46519797610000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-0.11741038400000001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-1.1899872000000001E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-4.6945969999999997E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-6.2428892E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-6.5254820000000005E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-0.3440744805</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.7078124999999998E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.0339425E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-7.239864E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-0.25406944599999998</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.358475818</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-0.2369608</v>
+      </c>
+      <c r="C5" s="4">
+        <v>-0.23634328600000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-0.110638029</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-6.7605090000000007E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.4587014000000001E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-0.48653523199999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-0.18846595899999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.48376035299999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.15634816400000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-0.10476158000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.27767718000000002</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-0.12641769899999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-0.1713894785</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.8864749999999998E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.2698443000000001E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-4.3041280000000001E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-7.8774517000000002E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8.2550703000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-0.131122566</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.52267280900000002</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.14700364099999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-5.5415689999999997E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.239450263</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-0.115756189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-7.4830987900000007E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.3319189999999999E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.6648044999999997E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-1.516231E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-2.1005630000000002E-3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4.8161047999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-5.1624946999999997E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.17512698199999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7.6770253999999996E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.57867928999999996</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.286296834</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-0.17971151799999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-4.6668096300000003E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5.6914620999999999E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-0.16427930700000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-4.9587659999999999E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9.8179812000000005E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.6327528000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-2.6243220500000001E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.1212795000000003E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-4.7374990999999998E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.122193E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.7977406999999999E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4.8806780000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.45493388E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.8813422000000002E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-6.3721088999999995E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.7271260000000001E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.1668471000000002E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.7594359999999997E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-2.0607748999999999E-3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.17413403899999999</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-8.3532041000000001E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.10306187999999999</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-3.5652243E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>8.4352883000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-1.1150263E-3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7.3928353000000002E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-8.3787590999999995E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-0.2303074</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-0.20564406099999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-0.21017197000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.998203E-4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9.9003249999999998E-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-1.303074E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1.060636E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-1.9049408E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-4.7152468000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5.4710434000000002E-3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.151421999</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-9.7447290000000006E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-0.22224345000000001</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-0.20124312999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-0.24298362000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.67279174E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-0.20987341500000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.64472713299999995</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-3.4859299999999999E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7.5932320000000001E-3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-6.5670746000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.7713524299999998E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-6.6694012999999996E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>8.8110108000000006E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7.2264259999999997E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4.3263478000000001E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>6.4796257999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.3664657499999998E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-0.214197479</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.64619242399999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>-1.1271059999999999E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.778825E-3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-6.0063233000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5.7647318199999999E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.16339051800000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8.6448382000000004E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-0.31256550999999999</v>
+      </c>
+      <c r="F21" s="3">
+        <v>-0.47571312300000002</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-0.161380367</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1">
+        <v>7.18907882E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-0.20800448299999999</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-1.6784707999999999E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>-0.59658840000000002</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.253923546</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.17015984200000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>9.8879556600000001E-2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>-0.240598117</v>
+      </c>
+      <c r="D23" s="3">
+        <v>-0.13587717999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.310216E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-0.30576797999999999</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.6978592000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.16018293210000001</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.18957714000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7.3373753999999999E-2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>7.4261439999999998E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-2.1799984000000001E-2</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.49085000699999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.3040951744</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.20450646</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.7665723000000006E-2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-0.21612387</v>
+      </c>
+      <c r="F25" s="3">
+        <v>-0.39597657200000003</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-3.6143762000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.39608138250000002</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-6.8983222999999996E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-6.5690594000000005E-2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>8.6183979999999993E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.26294779299999999</v>
+      </c>
+      <c r="G26" s="3">
+        <v>-0.36689286700000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="H31" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H33" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G31" xr:uid="{53F67C65-8765-BE4A-A3F4-4849C74ABCB4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">
+      <sortCondition ref="B1:B32"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final model with just variables (no pc's)
</commit_message>
<xml_diff>
--- a/PCA_layout_for_naming.xlsx
+++ b/PCA_layout_for_naming.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaacjohnson/Documents/Scanner Output/School/Willamette/Machine Learning/Week 10/Project 2/Git_Project2/ML-Project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Documents\Schooling\Willamette-MSDS\2-DATA505_MachineLearning\Project_2\repo\ML-Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21E8D84-CB08-1A4D-A2DD-727F584DDBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B110C2D-B1A7-42E9-82F9-EF1CBC5F5834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26700" windowHeight="16920" activeTab="1" xr2:uid="{7BAF7EC1-6934-4E82-A88D-5BFC29E54102}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BAF7EC1-6934-4E82-A88D-5BFC29E54102}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
     <sheet name="v2" sheetId="2" r:id="rId2"/>
+    <sheet name="v3(continuous)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'v2'!$A$1:$G$31</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t>PC1</t>
   </si>
@@ -277,6 +278,18 @@
   </si>
   <si>
     <t>income/gender?</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>- Total_Ct_Chng_Q4_Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Total_Revolving_Bal</t>
   </si>
 </sst>
 </file>
@@ -286,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +317,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -353,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -364,7 +383,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,23 +699,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49EB4EE4-2F6D-4B8C-8F30-3514F7F0C1A4}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -740,7 +758,7 @@
         <v>-6.0063233000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -763,7 +781,7 @@
         <v>1.6327528000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -786,7 +804,7 @@
         <v>-6.5670746000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -809,7 +827,7 @@
         <v>1.6978592000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -832,7 +850,7 @@
         <v>6.4796257999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -855,7 +873,7 @@
         <v>8.4352883000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -878,7 +896,7 @@
         <v>-6.5254820000000005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -901,7 +919,7 @@
         <v>-0.161380367</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -924,7 +942,7 @@
         <v>-5.0773237999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -947,7 +965,7 @@
         <v>-0.21017197000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -970,7 +988,7 @@
         <v>-0.12641769899999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -993,7 +1011,7 @@
         <v>-0.115756189</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1016,7 +1034,7 @@
         <v>-0.24298362000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1057,7 @@
         <v>-3.6143762000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1062,7 +1080,7 @@
         <v>-0.48653523199999998</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1085,7 +1103,7 @@
         <v>0.17015984200000001</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1126,7 @@
         <v>-0.17971151799999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>5.7594359999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1154,7 +1172,7 @@
         <v>4.8806780000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1177,7 +1195,7 @@
         <v>-0.36689286700000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1200,7 +1218,7 @@
         <v>8.2550703000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1223,7 +1241,7 @@
         <v>0.358475818</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1246,7 +1264,7 @@
         <v>4.8161047999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1269,7 +1287,7 @@
         <v>-4.7152468000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1292,14 +1310,14 @@
         <v>0.49085000699999998</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="H27" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1325,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1351,7 +1369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
@@ -1397,12 +1415,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H32" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -1422,71 +1440,71 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
     </row>
   </sheetData>
@@ -1502,22 +1520,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F67C65-8765-BE4A-A3F4-4849C74ABCB4}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G27" sqref="G27:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="23.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1560,7 +1578,7 @@
         <v>-5.0773237999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>-6.5254820000000005E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1606,7 +1624,7 @@
         <v>0.358475818</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1629,7 +1647,7 @@
         <v>-0.48653523199999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>-0.12641769899999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1675,7 +1693,7 @@
         <v>8.2550703000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1698,7 +1716,7 @@
         <v>-0.115756189</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1721,7 +1739,7 @@
         <v>4.8161047999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1744,7 +1762,7 @@
         <v>-0.17971151799999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1767,7 +1785,7 @@
         <v>1.6327528000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>4.8806780000000003E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1813,7 +1831,7 @@
         <v>5.7594359999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1854,7 @@
         <v>8.4352883000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1859,7 +1877,7 @@
         <v>-0.21017197000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1882,7 +1900,7 @@
         <v>-4.7152468000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1905,7 +1923,7 @@
         <v>-0.24298362000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1946,7 @@
         <v>-6.5670746000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1969,7 @@
         <v>6.4796257999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +1992,7 @@
         <v>-6.0063233000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1997,7 +2015,7 @@
         <v>-0.161380367</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2020,7 +2038,7 @@
         <v>0.17015984200000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2043,7 +2061,7 @@
         <v>1.6978592000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2066,7 +2084,7 @@
         <v>0.49085000699999998</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>-3.6143762000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2112,7 +2130,7 @@
         <v>-0.36689286700000001</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2138,11 +2156,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C28" t="s">
@@ -2164,7 +2182,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2190,7 +2208,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -2216,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2226,17 +2244,17 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H32" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H33" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -2256,71 +2274,71 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
     </row>
   </sheetData>
@@ -2331,4 +2349,562 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC57C12-E789-45EC-B2C4-D3C1785E8EE7}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>4.4529873999999997E-2</v>
+      </c>
+      <c r="C2">
+        <v>-0.27119934000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.62978769400000001</v>
+      </c>
+      <c r="E2">
+        <v>-5.0434069999999998E-2</v>
+      </c>
+      <c r="F2">
+        <v>4.4529873999999997E-2</v>
+      </c>
+      <c r="G2">
+        <v>-0.27119934000000001</v>
+      </c>
+      <c r="H2">
+        <v>0.62978769400000001</v>
+      </c>
+      <c r="I2">
+        <v>-5.0434069999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>-8.1101474000000007E-2</v>
+      </c>
+      <c r="C3">
+        <v>7.8021770000000004E-2</v>
+      </c>
+      <c r="D3">
+        <v>-0.14891702600000001</v>
+      </c>
+      <c r="E3">
+        <v>3.9235869999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>-8.1101474000000007E-2</v>
+      </c>
+      <c r="G3">
+        <v>7.8021770000000004E-2</v>
+      </c>
+      <c r="H3">
+        <v>-0.14891702600000001</v>
+      </c>
+      <c r="I3">
+        <v>3.9235869999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3.5944775999999998E-2</v>
+      </c>
+      <c r="C4">
+        <v>-0.26877095000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.62955033100000002</v>
+      </c>
+      <c r="E4">
+        <v>-4.8137880000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>3.5944775999999998E-2</v>
+      </c>
+      <c r="G4">
+        <v>-0.26877095000000001</v>
+      </c>
+      <c r="H4">
+        <v>0.62955033100000002</v>
+      </c>
+      <c r="I4">
+        <v>-4.8137880000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.174268688</v>
+      </c>
+      <c r="C5">
+        <v>-0.22869934</v>
+      </c>
+      <c r="D5">
+        <v>-0.170687219</v>
+      </c>
+      <c r="E5">
+        <v>-0.28149107000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.174268688</v>
+      </c>
+      <c r="G5">
+        <v>-0.22869934</v>
+      </c>
+      <c r="H5">
+        <v>-0.170687219</v>
+      </c>
+      <c r="I5">
+        <v>-0.28149107000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>2.3157212999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>-9.5799430000000005E-2</v>
+      </c>
+      <c r="D6">
+        <v>6.9405623E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.10243141</v>
+      </c>
+      <c r="F6">
+        <v>2.3157212999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>-9.5799430000000005E-2</v>
+      </c>
+      <c r="H6">
+        <v>6.9405623E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.10243141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1.3938625E-2</v>
+      </c>
+      <c r="C7">
+        <v>-0.19397528</v>
+      </c>
+      <c r="D7">
+        <v>-0.120292103</v>
+      </c>
+      <c r="E7">
+        <v>4.7043840000000003E-2</v>
+      </c>
+      <c r="F7">
+        <v>1.3938625E-2</v>
+      </c>
+      <c r="G7">
+        <v>-0.19397528</v>
+      </c>
+      <c r="H7">
+        <v>-0.120292103</v>
+      </c>
+      <c r="I7">
+        <v>4.7043840000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>-0.53826030999999996</v>
+      </c>
+      <c r="C8">
+        <v>-0.14187739999999999</v>
+      </c>
+      <c r="D8">
+        <v>-8.3735749999999994E-3</v>
+      </c>
+      <c r="E8">
+        <v>-0.26900596999999998</v>
+      </c>
+      <c r="F8">
+        <v>-0.53826030999999996</v>
+      </c>
+      <c r="G8">
+        <v>-0.14187739999999999</v>
+      </c>
+      <c r="H8">
+        <v>-8.3735749999999994E-3</v>
+      </c>
+      <c r="I8">
+        <v>-0.26900596999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.15984235299999999</v>
+      </c>
+      <c r="C9">
+        <v>0.25632061</v>
+      </c>
+      <c r="D9">
+        <v>0.14062754899999999</v>
+      </c>
+      <c r="E9">
+        <v>-0.36918604999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.15984235299999999</v>
+      </c>
+      <c r="G9">
+        <v>0.25632061</v>
+      </c>
+      <c r="H9">
+        <v>0.14062754899999999</v>
+      </c>
+      <c r="I9">
+        <v>-0.36918604999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>-0.55247729400000001</v>
+      </c>
+      <c r="C10">
+        <v>-0.16482696999999999</v>
+      </c>
+      <c r="D10">
+        <v>-2.0979191000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>-0.23585165999999999</v>
+      </c>
+      <c r="F10">
+        <v>-0.55247729400000001</v>
+      </c>
+      <c r="G10">
+        <v>-0.16482696999999999</v>
+      </c>
+      <c r="H10">
+        <v>-2.0979191000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>-0.23585165999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>5.5264090000000004E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.14156252</v>
+      </c>
+      <c r="D11">
+        <v>-4.3934833999999999E-2</v>
+      </c>
+      <c r="E11">
+        <v>-0.53503294000000001</v>
+      </c>
+      <c r="F11">
+        <v>5.5264090000000004E-3</v>
+      </c>
+      <c r="G11">
+        <v>0.14156252</v>
+      </c>
+      <c r="H11">
+        <v>-4.3934833999999999E-2</v>
+      </c>
+      <c r="I11">
+        <v>-0.53503294000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>-0.296696758</v>
+      </c>
+      <c r="C12">
+        <v>0.48408971000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.232165222</v>
+      </c>
+      <c r="E12">
+        <v>0.16561275</v>
+      </c>
+      <c r="F12">
+        <v>-0.296696758</v>
+      </c>
+      <c r="G12">
+        <v>0.48408971000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.232165222</v>
+      </c>
+      <c r="I12">
+        <v>0.16561275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>-0.231386757</v>
+      </c>
+      <c r="C13">
+        <v>0.50924095999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.21721633400000001</v>
+      </c>
+      <c r="E13">
+        <v>0.17603367</v>
+      </c>
+      <c r="F13">
+        <v>-0.231386757</v>
+      </c>
+      <c r="G13">
+        <v>0.50924095999999996</v>
+      </c>
+      <c r="H13">
+        <v>0.21721633400000001</v>
+      </c>
+      <c r="I13">
+        <v>0.17603367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>4.8487239999999996E-3</v>
+      </c>
+      <c r="C14">
+        <v>0.21000711</v>
+      </c>
+      <c r="D14">
+        <v>3.9881505999999997E-2</v>
+      </c>
+      <c r="E14">
+        <v>-0.51914875000000005</v>
+      </c>
+      <c r="F14">
+        <v>4.8487239999999996E-3</v>
+      </c>
+      <c r="G14">
+        <v>0.21000711</v>
+      </c>
+      <c r="H14">
+        <v>3.9881505999999997E-2</v>
+      </c>
+      <c r="I14">
+        <v>-0.51914875000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>0.44375640700000002</v>
+      </c>
+      <c r="C15">
+        <v>0.27965846</v>
+      </c>
+      <c r="D15">
+        <v>0.107449159</v>
+      </c>
+      <c r="E15">
+        <v>-0.15224156999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.44375640700000002</v>
+      </c>
+      <c r="G15">
+        <v>0.27965846</v>
+      </c>
+      <c r="H15">
+        <v>0.107449159</v>
+      </c>
+      <c r="I15">
+        <v>-0.15224156999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C23:E36">
+    <sortCondition descending="1" ref="C23:C36"/>
+  </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>